<commit_message>
configuracion subida de archivos
</commit_message>
<xml_diff>
--- a/archivo.xlsx
+++ b/archivo.xlsx
@@ -550,12 +550,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="1" max="1"/>
     <col width="40" customWidth="1" min="6" max="6"/>
     <col width="10" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="25" customWidth="1" min="12" max="12"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="45" customWidth="1" min="17" max="17"/>
   </cols>
@@ -574,7 +575,7 @@
       <c r="G1" s="3" t="n"/>
       <c r="I1" s="4" t="inlineStr">
         <is>
-          <t>BOGO-FONT-H-09-COS</t>
+          <t>MEDE-CABA-H-07-COS</t>
         </is>
       </c>
     </row>
@@ -717,7 +718,11 @@
       </c>
       <c r="J4" s="15" t="n"/>
       <c r="K4" s="15" t="n"/>
-      <c r="L4" s="15" t="n"/>
+      <c r="L4" s="15" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-07-COS</t>
+        </is>
+      </c>
       <c r="M4" s="15" t="n"/>
       <c r="N4" s="15" t="n"/>
       <c r="O4" s="15" t="n"/>
@@ -748,7 +753,11 @@
       <c r="I5" s="9" t="n"/>
       <c r="J5" s="16" t="n"/>
       <c r="K5" s="16" t="n"/>
-      <c r="L5" s="16" t="n"/>
+      <c r="L5" s="16" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-07-COS</t>
+        </is>
+      </c>
       <c r="M5" s="16" t="n"/>
       <c r="N5" s="16" t="n"/>
       <c r="O5" s="16" t="n"/>
@@ -802,7 +811,11 @@
       <c r="I7" s="16" t="n"/>
       <c r="J7" s="16" t="n"/>
       <c r="K7" s="16" t="n"/>
-      <c r="L7" s="16" t="n"/>
+      <c r="L7" s="16" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-07-COS</t>
+        </is>
+      </c>
       <c r="M7" s="16" t="n"/>
       <c r="N7" s="16" t="n"/>
       <c r="O7" s="16" t="n"/>
@@ -813,7 +826,11 @@
       <c r="I8" s="9" t="n"/>
       <c r="J8" s="15" t="n"/>
       <c r="K8" s="15" t="n"/>
-      <c r="L8" s="15" t="n"/>
+      <c r="L8" s="15" t="inlineStr">
+        <is>
+          <t>MEDE-CABA-H-07-COS</t>
+        </is>
+      </c>
       <c r="M8" s="15" t="n"/>
       <c r="N8" s="15" t="n"/>
       <c r="O8" s="15" t="n"/>
@@ -847,21 +864,21 @@
     <row r="20">
       <c r="F20" t="inlineStr">
         <is>
-          <t>interface upstream + add rest parts</t>
+          <t>interface upstream 0/18.0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="F21" t="inlineStr">
         <is>
-          <t>description PUERTO LIBRE</t>
+          <t xml:space="preserve">  description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="F22" t="inlineStr">
         <is>
-          <t>logical-channel 0 description PUERTO LIBRE</t>
+          <t xml:space="preserve">  logical-channel 0 description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
@@ -875,21 +892,21 @@
     <row r="24">
       <c r="F24" t="inlineStr">
         <is>
-          <t>interface upstream + add rest parts</t>
+          <t>interface upstream 0/18.1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="F25" t="inlineStr">
         <is>
-          <t>description PUERTO LIBRE</t>
+          <t xml:space="preserve">  description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="F26" t="inlineStr">
         <is>
-          <t>logical-channel 0 description PUERTO LIBRE</t>
+          <t xml:space="preserve">  logical-channel 0 description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
@@ -903,21 +920,21 @@
     <row r="28">
       <c r="F28" t="inlineStr">
         <is>
-          <t>interface upstream + add rest parts</t>
+          <t>interface upstream 0/18.2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="F29" t="inlineStr">
         <is>
-          <t>description PUERTO LIBRE</t>
+          <t xml:space="preserve">  description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="F30" t="inlineStr">
         <is>
-          <t>logical-channel 0 description PUERTO LIBRE</t>
+          <t xml:space="preserve">  logical-channel 0 description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
@@ -931,21 +948,21 @@
     <row r="32">
       <c r="F32" t="inlineStr">
         <is>
-          <t>interface upstream + add rest parts</t>
+          <t>interface upstream 0/18.3</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="F33" t="inlineStr">
         <is>
-          <t>description PUERTO LIBRE</t>
+          <t xml:space="preserve">  description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="F34" t="inlineStr">
         <is>
-          <t>logical-channel 0 description PUERTO LIBRE</t>
+          <t xml:space="preserve">  logical-channel 0 description "PUERTO LIBRE"</t>
         </is>
       </c>
     </row>
@@ -959,7 +976,7 @@
     <row r="39">
       <c r="F39" t="inlineStr">
         <is>
-          <t>no service group + add rests parts less</t>
+          <t xml:space="preserve">no service group  IRL </t>
         </is>
       </c>
     </row>
@@ -973,7 +990,7 @@
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="G4:G8"/>
+    <mergeCell ref="G4:G7"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="I1:Q1"/>
     <mergeCell ref="I2:Q2"/>

</xml_diff>